<commit_message>
add new data and broker akumulator
</commit_message>
<xml_diff>
--- a/public/data/netprofit-saham.xlsx
+++ b/public/data/netprofit-saham.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="11460"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2698" uniqueCount="2032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="2073">
   <si>
     <t>No</t>
   </si>
@@ -5255,6 +5255,21 @@
     <t>PLIN</t>
   </si>
   <si>
+    <t>726000000000</t>
+  </si>
+  <si>
+    <t>549000000000</t>
+  </si>
+  <si>
+    <t>557000000000</t>
+  </si>
+  <si>
+    <t>613000000000</t>
+  </si>
+  <si>
+    <t>998000000000</t>
+  </si>
+  <si>
     <t>PMJS</t>
   </si>
   <si>
@@ -5267,6 +5282,30 @@
     <t>PNBN</t>
   </si>
   <si>
+    <t>2518000000000</t>
+  </si>
+  <si>
+    <t>3187000000000</t>
+  </si>
+  <si>
+    <t>3498000000000</t>
+  </si>
+  <si>
+    <t>3124000000000</t>
+  </si>
+  <si>
+    <t>1817000000000</t>
+  </si>
+  <si>
+    <t>3273000000000</t>
+  </si>
+  <si>
+    <t>3006000000000</t>
+  </si>
+  <si>
+    <t>2867000000000</t>
+  </si>
+  <si>
     <t>PNBS</t>
   </si>
   <si>
@@ -5276,9 +5315,54 @@
     <t>PNIN</t>
   </si>
   <si>
+    <t>2395000000000</t>
+  </si>
+  <si>
+    <t>1863000000000</t>
+  </si>
+  <si>
+    <t>2140000000000</t>
+  </si>
+  <si>
+    <t>2293000000000</t>
+  </si>
+  <si>
+    <t>1929000000000</t>
+  </si>
+  <si>
+    <t>1486000000000</t>
+  </si>
+  <si>
+    <t>2404000000000</t>
+  </si>
+  <si>
+    <t>3542000000000</t>
+  </si>
+  <si>
     <t>PNLF</t>
   </si>
   <si>
+    <t>1678000000000</t>
+  </si>
+  <si>
+    <t>1609000000000</t>
+  </si>
+  <si>
+    <t>1993000000000</t>
+  </si>
+  <si>
+    <t>1496000000000</t>
+  </si>
+  <si>
+    <t>1985000000000</t>
+  </si>
+  <si>
+    <t>3607000000000</t>
+  </si>
+  <si>
+    <t>3457000000000</t>
+  </si>
+  <si>
     <t>PNSE</t>
   </si>
   <si>
@@ -5291,6 +5375,9 @@
     <t>POLL</t>
   </si>
   <si>
+    <t>469000000000</t>
+  </si>
+  <si>
     <t>POLU</t>
   </si>
   <si>
@@ -5309,28 +5396,64 @@
     <t>POWR</t>
   </si>
   <si>
+    <t>1382000000000</t>
+  </si>
+  <si>
+    <t>1437000000000</t>
+  </si>
+  <si>
+    <t>1124000000000</t>
+  </si>
+  <si>
+    <t>1090000000000</t>
+  </si>
+  <si>
+    <t>1294000000000</t>
+  </si>
+  <si>
+    <t>1079000000000</t>
+  </si>
+  <si>
+    <t>1174000000000</t>
+  </si>
+  <si>
     <t>PPGL</t>
   </si>
   <si>
     <t>PPRE</t>
   </si>
   <si>
+    <t>432000000000</t>
+  </si>
+  <si>
+    <t>439000000000</t>
+  </si>
+  <si>
     <t>PPRI</t>
   </si>
   <si>
     <t>PPRO</t>
   </si>
   <si>
+    <t>497000000000</t>
+  </si>
+  <si>
     <t>PRAY</t>
   </si>
   <si>
     <t>PRDA</t>
   </si>
   <si>
+    <t>622000000000</t>
+  </si>
+  <si>
     <t>PRIM</t>
   </si>
   <si>
     <t>PSAB</t>
+  </si>
+  <si>
+    <t>273000000000</t>
   </si>
   <si>
     <t>PSAT</t>
@@ -7160,8 +7283,8 @@
   <sheetPr/>
   <dimension ref="A1:AY958"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A669" workbookViewId="0">
-      <selection activeCell="C682" sqref="C682"/>
+    <sheetView tabSelected="1" topLeftCell="A685" workbookViewId="0">
+      <selection activeCell="C717" sqref="C717"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -40245,12 +40368,24 @@
       <c r="C683" s="2"/>
       <c r="D683" s="2"/>
       <c r="E683" s="2"/>
-      <c r="F683" s="2"/>
-      <c r="G683" s="2"/>
-      <c r="H683" s="2"/>
-      <c r="I683" s="2"/>
-      <c r="J683" s="2"/>
-      <c r="K683" s="2"/>
+      <c r="F683" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="G683" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="H683" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="I683" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="J683" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="K683" s="2">
+        <v>0</v>
+      </c>
       <c r="L683" s="2"/>
       <c r="M683" s="2"/>
       <c r="N683" s="2"/>
@@ -40275,15 +40410,33 @@
       <c r="B684" s="2" t="s">
         <v>1737</v>
       </c>
-      <c r="C684" s="2"/>
-      <c r="D684" s="2"/>
-      <c r="E684" s="2"/>
-      <c r="F684" s="2"/>
-      <c r="G684" s="2"/>
-      <c r="H684" s="2"/>
-      <c r="I684" s="2"/>
-      <c r="J684" s="2"/>
-      <c r="K684" s="2"/>
+      <c r="C684" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D684" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="E684" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="F684" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="G684" s="2">
+        <v>-394000000000</v>
+      </c>
+      <c r="H684" s="2">
+        <v>-276000000000</v>
+      </c>
+      <c r="I684" s="5" t="s">
+        <v>1520</v>
+      </c>
+      <c r="J684" s="5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="K684" s="5" t="s">
+        <v>1228</v>
+      </c>
       <c r="L684" s="2"/>
       <c r="M684" s="2"/>
       <c r="N684" s="2"/>
@@ -40308,15 +40461,33 @@
       <c r="B685" s="2" t="s">
         <v>1738</v>
       </c>
-      <c r="C685" s="2"/>
-      <c r="D685" s="2"/>
-      <c r="E685" s="2"/>
-      <c r="F685" s="2"/>
-      <c r="G685" s="2"/>
-      <c r="H685" s="2"/>
-      <c r="I685" s="2"/>
-      <c r="J685" s="2"/>
-      <c r="K685" s="2"/>
+      <c r="C685" s="2">
+        <v>-14000000000</v>
+      </c>
+      <c r="D685" s="2">
+        <v>-10000000000</v>
+      </c>
+      <c r="E685" s="2">
+        <v>-4000000000</v>
+      </c>
+      <c r="F685" s="2">
+        <v>-41000000000</v>
+      </c>
+      <c r="G685" s="2">
+        <v>0</v>
+      </c>
+      <c r="H685" s="2">
+        <v>-1000000000</v>
+      </c>
+      <c r="I685" s="2">
+        <v>-29000000000</v>
+      </c>
+      <c r="J685" s="2">
+        <v>-6000000000</v>
+      </c>
+      <c r="K685" s="2">
+        <v>16000000000</v>
+      </c>
       <c r="L685" s="2"/>
       <c r="M685" s="2"/>
       <c r="N685" s="2"/>
@@ -40344,12 +40515,24 @@
       <c r="C686" s="2"/>
       <c r="D686" s="2"/>
       <c r="E686" s="2"/>
-      <c r="F686" s="2"/>
-      <c r="G686" s="2"/>
-      <c r="H686" s="2"/>
-      <c r="I686" s="2"/>
-      <c r="J686" s="2"/>
-      <c r="K686" s="2"/>
+      <c r="F686" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="G686" s="2">
+        <v>0</v>
+      </c>
+      <c r="H686" s="2">
+        <v>-1000000000</v>
+      </c>
+      <c r="I686" s="2">
+        <v>-2000000000</v>
+      </c>
+      <c r="J686" s="2">
+        <v>-1000000000</v>
+      </c>
+      <c r="K686" s="2">
+        <v>-1000000000</v>
+      </c>
       <c r="L686" s="2"/>
       <c r="M686" s="2"/>
       <c r="N686" s="2"/>
@@ -40374,10 +40557,18 @@
       <c r="B687" s="2" t="s">
         <v>1740</v>
       </c>
-      <c r="C687" s="2"/>
-      <c r="D687" s="2"/>
-      <c r="E687" s="2"/>
-      <c r="F687" s="2"/>
+      <c r="C687" s="2">
+        <v>-19000000000</v>
+      </c>
+      <c r="D687" s="2">
+        <v>-14000000000</v>
+      </c>
+      <c r="E687" s="2">
+        <v>0</v>
+      </c>
+      <c r="F687" s="2">
+        <v>0</v>
+      </c>
       <c r="G687" s="2"/>
       <c r="H687" s="2"/>
       <c r="I687" s="2"/>
@@ -40407,15 +40598,33 @@
       <c r="B688" s="2" t="s">
         <v>1741</v>
       </c>
-      <c r="C688" s="2"/>
-      <c r="D688" s="2"/>
-      <c r="E688" s="2"/>
-      <c r="F688" s="2"/>
-      <c r="G688" s="2"/>
-      <c r="H688" s="2"/>
-      <c r="I688" s="2"/>
-      <c r="J688" s="2"/>
-      <c r="K688" s="2"/>
+      <c r="C688" s="5" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D688" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E688" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F688" s="5" t="s">
+        <v>1743</v>
+      </c>
+      <c r="G688" s="2">
+        <v>-575000000000</v>
+      </c>
+      <c r="H688" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="I688" s="5" t="s">
+        <v>1744</v>
+      </c>
+      <c r="J688" s="5" t="s">
+        <v>1745</v>
+      </c>
+      <c r="K688" s="5" t="s">
+        <v>1746</v>
+      </c>
       <c r="L688" s="2"/>
       <c r="M688" s="2"/>
       <c r="N688" s="2"/>
@@ -40438,17 +40647,31 @@
         <v>688</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>1742</v>
+        <v>1747</v>
       </c>
       <c r="C689" s="2"/>
       <c r="D689" s="2"/>
-      <c r="E689" s="2"/>
-      <c r="F689" s="2"/>
-      <c r="G689" s="2"/>
-      <c r="H689" s="2"/>
-      <c r="I689" s="2"/>
-      <c r="J689" s="2"/>
-      <c r="K689" s="2"/>
+      <c r="E689" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="F689" s="5" t="s">
+        <v>1620</v>
+      </c>
+      <c r="G689" s="2">
+        <v>69000000000</v>
+      </c>
+      <c r="H689" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="I689" s="5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J689" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K689" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="L689" s="2"/>
       <c r="M689" s="2"/>
       <c r="N689" s="2"/>
@@ -40471,16 +40694,30 @@
         <v>689</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1743</v>
+        <v>1748</v>
       </c>
       <c r="C690" s="2"/>
-      <c r="D690" s="2"/>
-      <c r="E690" s="2"/>
-      <c r="F690" s="2"/>
-      <c r="G690" s="2"/>
-      <c r="H690" s="2"/>
-      <c r="I690" s="2"/>
-      <c r="J690" s="2"/>
+      <c r="D690" s="2">
+        <v>64000000000</v>
+      </c>
+      <c r="E690" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="F690" s="2">
+        <v>81000000000</v>
+      </c>
+      <c r="G690" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="H690" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I690" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="J690" s="2">
+        <v>1000000000</v>
+      </c>
       <c r="K690" s="2"/>
       <c r="L690" s="2"/>
       <c r="M690" s="2"/>
@@ -40504,7 +40741,7 @@
         <v>690</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>1744</v>
+        <v>1749</v>
       </c>
       <c r="C691" s="2"/>
       <c r="D691" s="2"/>
@@ -40512,9 +40749,15 @@
       <c r="F691" s="2"/>
       <c r="G691" s="2"/>
       <c r="H691" s="2"/>
-      <c r="I691" s="2"/>
-      <c r="J691" s="2"/>
-      <c r="K691" s="2"/>
+      <c r="I691" s="2">
+        <v>26000000000</v>
+      </c>
+      <c r="J691" s="2">
+        <v>48000000000</v>
+      </c>
+      <c r="K691" s="2">
+        <v>50000000000</v>
+      </c>
       <c r="L691" s="2"/>
       <c r="M691" s="2"/>
       <c r="N691" s="2"/>
@@ -40537,17 +40780,35 @@
         <v>691</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C692" s="2"/>
-      <c r="D692" s="2"/>
-      <c r="E692" s="2"/>
-      <c r="F692" s="2"/>
-      <c r="G692" s="2"/>
-      <c r="H692" s="2"/>
-      <c r="I692" s="2"/>
-      <c r="J692" s="2"/>
-      <c r="K692" s="2"/>
+        <v>1750</v>
+      </c>
+      <c r="C692" s="5" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D692" s="5" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E692" s="5" t="s">
+        <v>1752</v>
+      </c>
+      <c r="F692" s="5" t="s">
+        <v>1753</v>
+      </c>
+      <c r="G692" s="5" t="s">
+        <v>1754</v>
+      </c>
+      <c r="H692" s="5" t="s">
+        <v>1755</v>
+      </c>
+      <c r="I692" s="5" t="s">
+        <v>1756</v>
+      </c>
+      <c r="J692" s="5" t="s">
+        <v>1757</v>
+      </c>
+      <c r="K692" s="5" t="s">
+        <v>1758</v>
+      </c>
       <c r="L692" s="2"/>
       <c r="M692" s="2"/>
       <c r="N692" s="2"/>
@@ -40570,17 +40831,35 @@
         <v>692</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C693" s="2"/>
-      <c r="D693" s="2"/>
-      <c r="E693" s="2"/>
-      <c r="F693" s="2"/>
-      <c r="G693" s="2"/>
-      <c r="H693" s="2"/>
-      <c r="I693" s="2"/>
-      <c r="J693" s="2"/>
-      <c r="K693" s="2"/>
+        <v>1759</v>
+      </c>
+      <c r="C693" s="2">
+        <v>20000000000</v>
+      </c>
+      <c r="D693" s="2">
+        <v>-969000000000</v>
+      </c>
+      <c r="E693" s="2">
+        <v>21000000000</v>
+      </c>
+      <c r="F693" s="2">
+        <v>13000000000</v>
+      </c>
+      <c r="G693" s="2">
+        <v>0</v>
+      </c>
+      <c r="H693" s="2">
+        <v>-818000000000</v>
+      </c>
+      <c r="I693" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="J693" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="K693" s="2">
+        <v>89000000000</v>
+      </c>
       <c r="L693" s="2"/>
       <c r="M693" s="2"/>
       <c r="N693" s="2"/>
@@ -40603,17 +40882,29 @@
         <v>693</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>1747</v>
+        <v>1760</v>
       </c>
       <c r="C694" s="2"/>
       <c r="D694" s="2"/>
       <c r="E694" s="2"/>
-      <c r="F694" s="2"/>
-      <c r="G694" s="2"/>
-      <c r="H694" s="2"/>
-      <c r="I694" s="2"/>
-      <c r="J694" s="2"/>
-      <c r="K694" s="2"/>
+      <c r="F694" s="2">
+        <v>21000000000</v>
+      </c>
+      <c r="G694" s="2">
+        <v>81000000000</v>
+      </c>
+      <c r="H694" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="I694" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J694" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="K694" s="5" t="s">
+        <v>495</v>
+      </c>
       <c r="L694" s="2"/>
       <c r="M694" s="2"/>
       <c r="N694" s="2"/>
@@ -40636,17 +40927,35 @@
         <v>694</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1748</v>
-      </c>
-      <c r="C695" s="2"/>
-      <c r="D695" s="2"/>
-      <c r="E695" s="2"/>
-      <c r="F695" s="2"/>
-      <c r="G695" s="2"/>
-      <c r="H695" s="2"/>
-      <c r="I695" s="2"/>
-      <c r="J695" s="2"/>
-      <c r="K695" s="2"/>
+        <v>1761</v>
+      </c>
+      <c r="C695" s="6" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D695" s="6" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E695" s="6" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F695" s="6" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G695" s="6" t="s">
+        <v>1766</v>
+      </c>
+      <c r="H695" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="I695" s="6" t="s">
+        <v>1768</v>
+      </c>
+      <c r="J695" s="6" t="s">
+        <v>1769</v>
+      </c>
+      <c r="K695" s="6" t="s">
+        <v>1049</v>
+      </c>
       <c r="L695" s="2"/>
       <c r="M695" s="2"/>
       <c r="N695" s="2"/>
@@ -40669,17 +40978,35 @@
         <v>695</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1749</v>
-      </c>
-      <c r="C696" s="2"/>
-      <c r="D696" s="2"/>
-      <c r="E696" s="2"/>
-      <c r="F696" s="2"/>
-      <c r="G696" s="2"/>
-      <c r="H696" s="2"/>
-      <c r="I696" s="2"/>
-      <c r="J696" s="2"/>
-      <c r="K696" s="2"/>
+        <v>1770</v>
+      </c>
+      <c r="C696" s="5" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D696" s="5" t="s">
+        <v>1772</v>
+      </c>
+      <c r="E696" s="5" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F696" s="5" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G696" s="5" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H696" s="5" t="s">
+        <v>1774</v>
+      </c>
+      <c r="I696" s="5" t="s">
+        <v>1775</v>
+      </c>
+      <c r="J696" s="5" t="s">
+        <v>1776</v>
+      </c>
+      <c r="K696" s="5" t="s">
+        <v>1777</v>
+      </c>
       <c r="L696" s="2"/>
       <c r="M696" s="2"/>
       <c r="N696" s="2"/>
@@ -40702,17 +41029,35 @@
         <v>696</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>1750</v>
-      </c>
-      <c r="C697" s="2"/>
-      <c r="D697" s="2"/>
-      <c r="E697" s="2"/>
-      <c r="F697" s="2"/>
-      <c r="G697" s="2"/>
-      <c r="H697" s="2"/>
-      <c r="I697" s="2"/>
-      <c r="J697" s="2"/>
-      <c r="K697" s="2"/>
+        <v>1778</v>
+      </c>
+      <c r="C697" s="2">
+        <v>-1000000000</v>
+      </c>
+      <c r="D697" s="2">
+        <v>28000000000</v>
+      </c>
+      <c r="E697" s="2">
+        <v>-10000000000</v>
+      </c>
+      <c r="F697" s="2">
+        <v>-14000000000</v>
+      </c>
+      <c r="G697" s="2">
+        <v>-51000000000</v>
+      </c>
+      <c r="H697" s="2">
+        <v>-42000000000</v>
+      </c>
+      <c r="I697" s="2">
+        <v>-13000000000</v>
+      </c>
+      <c r="J697" s="2">
+        <v>25000000000</v>
+      </c>
+      <c r="K697" s="2">
+        <v>11000000000</v>
+      </c>
       <c r="L697" s="2"/>
       <c r="M697" s="2"/>
       <c r="N697" s="2"/>
@@ -40735,17 +41080,33 @@
         <v>697</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>1751</v>
+        <v>1779</v>
       </c>
       <c r="C698" s="2"/>
-      <c r="D698" s="2"/>
-      <c r="E698" s="2"/>
-      <c r="F698" s="2"/>
-      <c r="G698" s="2"/>
-      <c r="H698" s="2"/>
-      <c r="I698" s="2"/>
-      <c r="J698" s="2"/>
-      <c r="K698" s="2"/>
+      <c r="D698" s="2">
+        <v>21000000000</v>
+      </c>
+      <c r="E698" s="2">
+        <v>30000000000</v>
+      </c>
+      <c r="F698" s="2">
+        <v>-55000000000</v>
+      </c>
+      <c r="G698" s="2">
+        <v>-38000000000</v>
+      </c>
+      <c r="H698" s="2">
+        <v>-47000000000</v>
+      </c>
+      <c r="I698" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="J698" s="2">
+        <v>-17000000000</v>
+      </c>
+      <c r="K698" s="2">
+        <v>-29000000000</v>
+      </c>
       <c r="L698" s="2"/>
       <c r="M698" s="2"/>
       <c r="N698" s="2"/>
@@ -40768,17 +41129,31 @@
         <v>698</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>1752</v>
+        <v>1780</v>
       </c>
       <c r="C699" s="2"/>
       <c r="D699" s="2"/>
-      <c r="E699" s="2"/>
-      <c r="F699" s="2"/>
-      <c r="G699" s="2"/>
-      <c r="H699" s="2"/>
-      <c r="I699" s="2"/>
-      <c r="J699" s="2"/>
-      <c r="K699" s="2"/>
+      <c r="E699" s="2">
+        <v>72000000000</v>
+      </c>
+      <c r="F699" s="2">
+        <v>55000000000</v>
+      </c>
+      <c r="G699" s="2">
+        <v>17000000000</v>
+      </c>
+      <c r="H699" s="2">
+        <v>36000000000</v>
+      </c>
+      <c r="I699" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="J699" s="2">
+        <v>92000000000</v>
+      </c>
+      <c r="K699" s="2">
+        <v>34000000000</v>
+      </c>
       <c r="L699" s="2"/>
       <c r="M699" s="2"/>
       <c r="N699" s="2"/>
@@ -40801,17 +41176,31 @@
         <v>699</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>1753</v>
+        <v>1781</v>
       </c>
       <c r="C700" s="2"/>
       <c r="D700" s="2"/>
-      <c r="E700" s="2"/>
-      <c r="F700" s="2"/>
-      <c r="G700" s="2"/>
-      <c r="H700" s="2"/>
-      <c r="I700" s="2"/>
-      <c r="J700" s="2"/>
-      <c r="K700" s="2"/>
+      <c r="E700" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F700" s="5" t="s">
+        <v>1652</v>
+      </c>
+      <c r="G700" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H700" s="2">
+        <v>86000000000</v>
+      </c>
+      <c r="I700" s="2">
+        <v>-137000000000</v>
+      </c>
+      <c r="J700" s="5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="K700" s="2">
+        <v>12000000000</v>
+      </c>
       <c r="L700" s="2"/>
       <c r="M700" s="2"/>
       <c r="N700" s="2"/>
@@ -40834,17 +41223,31 @@
         <v>700</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>1754</v>
+        <v>1783</v>
       </c>
       <c r="C701" s="2"/>
       <c r="D701" s="2"/>
-      <c r="E701" s="2"/>
-      <c r="F701" s="2"/>
-      <c r="G701" s="2"/>
-      <c r="H701" s="2"/>
-      <c r="I701" s="2"/>
-      <c r="J701" s="2"/>
-      <c r="K701" s="2"/>
+      <c r="E701" s="2">
+        <v>9000000000</v>
+      </c>
+      <c r="F701" s="2">
+        <v>9000000000</v>
+      </c>
+      <c r="G701" s="2">
+        <v>-6000000000</v>
+      </c>
+      <c r="H701" s="2">
+        <v>-52000000000</v>
+      </c>
+      <c r="I701" s="2">
+        <v>-6000000000</v>
+      </c>
+      <c r="J701" s="2">
+        <v>-15000000000</v>
+      </c>
+      <c r="K701" s="2">
+        <v>-1000000000</v>
+      </c>
       <c r="L701" s="2"/>
       <c r="M701" s="2"/>
       <c r="N701" s="2"/>
@@ -40867,17 +41270,35 @@
         <v>701</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C702" s="2"/>
-      <c r="D702" s="2"/>
-      <c r="E702" s="2"/>
-      <c r="F702" s="2"/>
-      <c r="G702" s="2"/>
-      <c r="H702" s="2"/>
-      <c r="I702" s="2"/>
-      <c r="J702" s="2"/>
-      <c r="K702" s="2"/>
+        <v>1784</v>
+      </c>
+      <c r="C702" s="2">
+        <v>-158000000000</v>
+      </c>
+      <c r="D702" s="2">
+        <v>-59000000000</v>
+      </c>
+      <c r="E702" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F702" s="2">
+        <v>-169000000000</v>
+      </c>
+      <c r="G702" s="2">
+        <v>-300000000000</v>
+      </c>
+      <c r="H702" s="2">
+        <v>24000000000</v>
+      </c>
+      <c r="I702" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J702" s="2">
+        <v>-515000000000</v>
+      </c>
+      <c r="K702" s="2">
+        <v>-769000000000</v>
+      </c>
       <c r="L702" s="2"/>
       <c r="M702" s="2"/>
       <c r="N702" s="2"/>
@@ -40900,14 +41321,26 @@
         <v>702</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C703" s="2"/>
-      <c r="D703" s="2"/>
-      <c r="E703" s="2"/>
-      <c r="F703" s="2"/>
-      <c r="G703" s="2"/>
-      <c r="H703" s="2"/>
+        <v>1785</v>
+      </c>
+      <c r="C703" s="2">
+        <v>19000000000</v>
+      </c>
+      <c r="D703" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E703" s="2">
+        <v>-61000000000</v>
+      </c>
+      <c r="F703" s="2">
+        <v>-419000000000</v>
+      </c>
+      <c r="G703" s="2">
+        <v>-82000000000</v>
+      </c>
+      <c r="H703" s="2">
+        <v>-155000000000</v>
+      </c>
       <c r="I703" s="2"/>
       <c r="J703" s="2"/>
       <c r="K703" s="2"/>
@@ -40933,17 +41366,35 @@
         <v>703</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C704" s="2"/>
-      <c r="D704" s="2"/>
-      <c r="E704" s="2"/>
-      <c r="F704" s="2"/>
-      <c r="G704" s="2"/>
-      <c r="H704" s="2"/>
-      <c r="I704" s="2"/>
-      <c r="J704" s="2"/>
-      <c r="K704" s="2"/>
+        <v>1786</v>
+      </c>
+      <c r="C704" s="2">
+        <v>94000000000</v>
+      </c>
+      <c r="D704" s="2">
+        <v>28000000000</v>
+      </c>
+      <c r="E704" s="2">
+        <v>-42000000000</v>
+      </c>
+      <c r="F704" s="2">
+        <v>-10000000000</v>
+      </c>
+      <c r="G704" s="2">
+        <v>-71000000000</v>
+      </c>
+      <c r="H704" s="2">
+        <v>-83000000000</v>
+      </c>
+      <c r="I704" s="2">
+        <v>17000000000</v>
+      </c>
+      <c r="J704" s="2">
+        <v>65000000000</v>
+      </c>
+      <c r="K704" s="2">
+        <v>-65000000000</v>
+      </c>
       <c r="L704" s="2"/>
       <c r="M704" s="2"/>
       <c r="N704" s="2"/>
@@ -40966,17 +41417,31 @@
         <v>704</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>1758</v>
+        <v>1787</v>
       </c>
       <c r="C705" s="2"/>
       <c r="D705" s="2"/>
-      <c r="E705" s="2"/>
-      <c r="F705" s="2"/>
-      <c r="G705" s="2"/>
-      <c r="H705" s="2"/>
-      <c r="I705" s="2"/>
-      <c r="J705" s="2"/>
-      <c r="K705" s="2"/>
+      <c r="E705" s="2">
+        <v>-353000000000</v>
+      </c>
+      <c r="F705" s="2">
+        <v>-151000000000</v>
+      </c>
+      <c r="G705" s="2">
+        <v>-136000000000</v>
+      </c>
+      <c r="H705" s="2">
+        <v>-141000000000</v>
+      </c>
+      <c r="I705" s="2">
+        <v>-122000000000</v>
+      </c>
+      <c r="J705" s="2">
+        <v>-146000000000</v>
+      </c>
+      <c r="K705" s="2">
+        <v>-120000000000</v>
+      </c>
       <c r="L705" s="2"/>
       <c r="M705" s="2"/>
       <c r="N705" s="2"/>
@@ -40999,17 +41464,35 @@
         <v>705</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>1759</v>
-      </c>
-      <c r="C706" s="2"/>
-      <c r="D706" s="2"/>
-      <c r="E706" s="2"/>
-      <c r="F706" s="2"/>
-      <c r="G706" s="2"/>
-      <c r="H706" s="2"/>
-      <c r="I706" s="2"/>
-      <c r="J706" s="2"/>
-      <c r="K706" s="2"/>
+        <v>1788</v>
+      </c>
+      <c r="C706" s="5" t="s">
+        <v>1789</v>
+      </c>
+      <c r="D706" s="5" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E706" s="5" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F706" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G706" s="5" t="s">
+        <v>1792</v>
+      </c>
+      <c r="H706" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="I706" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="J706" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="K706" s="5" t="s">
+        <v>1550</v>
+      </c>
       <c r="L706" s="2"/>
       <c r="M706" s="2"/>
       <c r="N706" s="2"/>
@@ -41032,17 +41515,29 @@
         <v>706</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>1760</v>
+        <v>1796</v>
       </c>
       <c r="C707" s="2"/>
       <c r="D707" s="2"/>
       <c r="E707" s="2"/>
-      <c r="F707" s="2"/>
-      <c r="G707" s="2"/>
-      <c r="H707" s="2"/>
-      <c r="I707" s="2"/>
-      <c r="J707" s="2"/>
-      <c r="K707" s="2"/>
+      <c r="F707" s="2">
+        <v>4000000000</v>
+      </c>
+      <c r="G707" s="2">
+        <v>7000000000</v>
+      </c>
+      <c r="H707" s="2">
+        <v>20000000000</v>
+      </c>
+      <c r="I707" s="2">
+        <v>20000000000</v>
+      </c>
+      <c r="J707" s="2">
+        <v>17000000000</v>
+      </c>
+      <c r="K707" s="2">
+        <v>13000000000</v>
+      </c>
       <c r="L707" s="2"/>
       <c r="M707" s="2"/>
       <c r="N707" s="2"/>
@@ -41065,17 +41560,35 @@
         <v>707</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>1761</v>
-      </c>
-      <c r="C708" s="2"/>
-      <c r="D708" s="2"/>
-      <c r="E708" s="2"/>
-      <c r="F708" s="2"/>
-      <c r="G708" s="2"/>
-      <c r="H708" s="2"/>
-      <c r="I708" s="2"/>
-      <c r="J708" s="2"/>
-      <c r="K708" s="2"/>
+        <v>1797</v>
+      </c>
+      <c r="C708" s="2">
+        <v>41000000000</v>
+      </c>
+      <c r="D708" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="E708" s="5" t="s">
+        <v>1798</v>
+      </c>
+      <c r="F708" s="5" t="s">
+        <v>1799</v>
+      </c>
+      <c r="G708" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H708" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="I708" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="J708" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K708" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="L708" s="2"/>
       <c r="M708" s="2"/>
       <c r="N708" s="2"/>
@@ -41098,17 +41611,27 @@
         <v>708</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>1762</v>
+        <v>1800</v>
       </c>
       <c r="C709" s="2"/>
       <c r="D709" s="2"/>
       <c r="E709" s="2"/>
       <c r="F709" s="2"/>
-      <c r="G709" s="2"/>
-      <c r="H709" s="2"/>
-      <c r="I709" s="2"/>
-      <c r="J709" s="2"/>
-      <c r="K709" s="2"/>
+      <c r="G709" s="2">
+        <v>0</v>
+      </c>
+      <c r="H709" s="2">
+        <v>3000000000</v>
+      </c>
+      <c r="I709" s="2">
+        <v>3000000000</v>
+      </c>
+      <c r="J709" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="K709" s="2">
+        <v>5000000000</v>
+      </c>
       <c r="L709" s="2"/>
       <c r="M709" s="2"/>
       <c r="N709" s="2"/>
@@ -41131,17 +41654,35 @@
         <v>709</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>1763</v>
-      </c>
-      <c r="C710" s="2"/>
-      <c r="D710" s="2"/>
-      <c r="E710" s="2"/>
-      <c r="F710" s="2"/>
-      <c r="G710" s="2"/>
-      <c r="H710" s="2"/>
-      <c r="I710" s="2"/>
-      <c r="J710" s="2"/>
-      <c r="K710" s="2"/>
+        <v>1801</v>
+      </c>
+      <c r="C710" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D710" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E710" s="5" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F710" s="5" t="s">
+        <v>1458</v>
+      </c>
+      <c r="G710" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="H710" s="2">
+        <v>21000000000</v>
+      </c>
+      <c r="I710" s="2">
+        <v>24000000000</v>
+      </c>
+      <c r="J710" s="2">
+        <v>-1284000000000</v>
+      </c>
+      <c r="K710" s="2">
+        <v>-1092000000000</v>
+      </c>
       <c r="L710" s="2"/>
       <c r="M710" s="2"/>
       <c r="N710" s="2"/>
@@ -41164,17 +41705,29 @@
         <v>710</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1764</v>
+        <v>1803</v>
       </c>
       <c r="C711" s="2"/>
       <c r="D711" s="2"/>
       <c r="E711" s="2"/>
-      <c r="F711" s="2"/>
-      <c r="G711" s="2"/>
-      <c r="H711" s="2"/>
-      <c r="I711" s="2"/>
-      <c r="J711" s="2"/>
-      <c r="K711" s="2"/>
+      <c r="F711" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G711" s="5" t="s">
+        <v>1596</v>
+      </c>
+      <c r="H711" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="I711" s="2">
+        <v>55000000000</v>
+      </c>
+      <c r="J711" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="K711" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="L711" s="2"/>
       <c r="M711" s="2"/>
       <c r="N711" s="2"/>
@@ -41197,17 +41750,35 @@
         <v>711</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1765</v>
-      </c>
-      <c r="C712" s="2"/>
-      <c r="D712" s="2"/>
-      <c r="E712" s="2"/>
-      <c r="F712" s="2"/>
-      <c r="G712" s="2"/>
-      <c r="H712" s="2"/>
-      <c r="I712" s="2"/>
-      <c r="J712" s="2"/>
-      <c r="K712" s="2"/>
+        <v>1804</v>
+      </c>
+      <c r="C712" s="2">
+        <v>88000000000</v>
+      </c>
+      <c r="D712" s="5" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E712" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F712" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="G712" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="H712" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="I712" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="J712" s="5" t="s">
+        <v>1350</v>
+      </c>
+      <c r="K712" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="L712" s="2"/>
       <c r="M712" s="2"/>
       <c r="N712" s="2"/>
@@ -41230,17 +41801,33 @@
         <v>712</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>1766</v>
+        <v>1806</v>
       </c>
       <c r="C713" s="2"/>
-      <c r="D713" s="2"/>
-      <c r="E713" s="2"/>
-      <c r="F713" s="2"/>
-      <c r="G713" s="2"/>
-      <c r="H713" s="2"/>
-      <c r="I713" s="2"/>
-      <c r="J713" s="2"/>
-      <c r="K713" s="2"/>
+      <c r="D713" s="2">
+        <v>20000000000</v>
+      </c>
+      <c r="E713" s="2">
+        <v>17000000000</v>
+      </c>
+      <c r="F713" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="G713" s="2">
+        <v>38000000000</v>
+      </c>
+      <c r="H713" s="2">
+        <v>75000000000</v>
+      </c>
+      <c r="I713" s="2">
+        <v>22000000000</v>
+      </c>
+      <c r="J713" s="2">
+        <v>-3000000000</v>
+      </c>
+      <c r="K713" s="2">
+        <v>-18000000000</v>
+      </c>
       <c r="L713" s="2"/>
       <c r="M713" s="2"/>
       <c r="N713" s="2"/>
@@ -41263,17 +41850,35 @@
         <v>713</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>1767</v>
-      </c>
-      <c r="C714" s="2"/>
-      <c r="D714" s="2"/>
-      <c r="E714" s="2"/>
-      <c r="F714" s="2"/>
-      <c r="G714" s="2"/>
-      <c r="H714" s="2"/>
-      <c r="I714" s="2"/>
-      <c r="J714" s="2"/>
-      <c r="K714" s="2"/>
+        <v>1807</v>
+      </c>
+      <c r="C714" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D714" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="E714" s="5" t="s">
+        <v>1808</v>
+      </c>
+      <c r="F714" s="2">
+        <v>59000000000</v>
+      </c>
+      <c r="G714" s="2">
+        <v>28000000000</v>
+      </c>
+      <c r="H714" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="I714" s="2">
+        <v>-239000000000</v>
+      </c>
+      <c r="J714" s="2">
+        <v>9000000000</v>
+      </c>
+      <c r="K714" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="L714" s="2"/>
       <c r="M714" s="2"/>
       <c r="N714" s="2"/>
@@ -41296,7 +41901,7 @@
         <v>714</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>1768</v>
+        <v>1809</v>
       </c>
       <c r="C715" s="2"/>
       <c r="D715" s="2"/>
@@ -41304,9 +41909,15 @@
       <c r="F715" s="2"/>
       <c r="G715" s="2"/>
       <c r="H715" s="2"/>
-      <c r="I715" s="2"/>
-      <c r="J715" s="2"/>
-      <c r="K715" s="2"/>
+      <c r="I715" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J715" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="K715" s="5" t="s">
+        <v>1448</v>
+      </c>
       <c r="L715" s="2"/>
       <c r="M715" s="2"/>
       <c r="N715" s="2"/>
@@ -41329,17 +41940,35 @@
         <v>715</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>1769</v>
-      </c>
-      <c r="C716" s="2"/>
-      <c r="D716" s="2"/>
-      <c r="E716" s="2"/>
-      <c r="F716" s="2"/>
-      <c r="G716" s="2"/>
-      <c r="H716" s="2"/>
-      <c r="I716" s="2"/>
-      <c r="J716" s="2"/>
-      <c r="K716" s="2"/>
+        <v>1810</v>
+      </c>
+      <c r="C716" s="2">
+        <v>-37000000000</v>
+      </c>
+      <c r="D716" s="2">
+        <v>32000000000</v>
+      </c>
+      <c r="E716" s="2">
+        <v>-47000000000</v>
+      </c>
+      <c r="F716" s="2">
+        <v>-26000000000</v>
+      </c>
+      <c r="G716" s="2">
+        <v>-52000000000</v>
+      </c>
+      <c r="H716" s="2">
+        <v>-81000000000</v>
+      </c>
+      <c r="I716" s="2">
+        <v>-26000000000</v>
+      </c>
+      <c r="J716" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="K716" s="2">
+        <v>-21000000000</v>
+      </c>
       <c r="L716" s="2"/>
       <c r="M716" s="2"/>
       <c r="N716" s="2"/>
@@ -41362,7 +41991,7 @@
         <v>716</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1770</v>
+        <v>1811</v>
       </c>
       <c r="C717" s="2"/>
       <c r="D717" s="2"/>
@@ -41395,7 +42024,7 @@
         <v>717</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>1771</v>
+        <v>1812</v>
       </c>
       <c r="C718" s="2"/>
       <c r="D718" s="2"/>
@@ -41428,7 +42057,7 @@
         <v>718</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>1772</v>
+        <v>1813</v>
       </c>
       <c r="C719" s="2"/>
       <c r="D719" s="2"/>
@@ -41461,7 +42090,7 @@
         <v>719</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>1773</v>
+        <v>1814</v>
       </c>
       <c r="C720" s="2"/>
       <c r="D720" s="2"/>
@@ -41494,7 +42123,7 @@
         <v>720</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>1774</v>
+        <v>1815</v>
       </c>
       <c r="C721" s="2"/>
       <c r="D721" s="2"/>
@@ -41527,7 +42156,7 @@
         <v>721</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>1775</v>
+        <v>1816</v>
       </c>
       <c r="C722" s="2"/>
       <c r="D722" s="2"/>
@@ -41560,7 +42189,7 @@
         <v>722</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>1776</v>
+        <v>1817</v>
       </c>
       <c r="C723" s="2"/>
       <c r="D723" s="2"/>
@@ -41593,7 +42222,7 @@
         <v>723</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>1777</v>
+        <v>1818</v>
       </c>
       <c r="C724" s="2"/>
       <c r="D724" s="2"/>
@@ -41626,7 +42255,7 @@
         <v>724</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>1778</v>
+        <v>1819</v>
       </c>
       <c r="C725" s="2"/>
       <c r="D725" s="2"/>
@@ -41659,7 +42288,7 @@
         <v>725</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>1779</v>
+        <v>1820</v>
       </c>
       <c r="C726" s="2"/>
       <c r="D726" s="2"/>
@@ -41692,7 +42321,7 @@
         <v>726</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>1780</v>
+        <v>1821</v>
       </c>
       <c r="C727" s="2"/>
       <c r="D727" s="2"/>
@@ -41725,7 +42354,7 @@
         <v>727</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>1781</v>
+        <v>1822</v>
       </c>
       <c r="C728" s="2"/>
       <c r="D728" s="2"/>
@@ -41758,7 +42387,7 @@
         <v>728</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1782</v>
+        <v>1823</v>
       </c>
       <c r="C729" s="2"/>
       <c r="D729" s="2"/>
@@ -41791,7 +42420,7 @@
         <v>729</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>1783</v>
+        <v>1824</v>
       </c>
       <c r="C730" s="2"/>
       <c r="D730" s="2"/>
@@ -41824,7 +42453,7 @@
         <v>730</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>1784</v>
+        <v>1825</v>
       </c>
       <c r="C731" s="2"/>
       <c r="D731" s="2"/>
@@ -41857,7 +42486,7 @@
         <v>731</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>1785</v>
+        <v>1826</v>
       </c>
       <c r="C732" s="2"/>
       <c r="D732" s="2"/>
@@ -41890,7 +42519,7 @@
         <v>732</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>1786</v>
+        <v>1827</v>
       </c>
       <c r="C733" s="2"/>
       <c r="D733" s="2"/>
@@ -41923,7 +42552,7 @@
         <v>733</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>1787</v>
+        <v>1828</v>
       </c>
       <c r="C734" s="2"/>
       <c r="D734" s="2"/>
@@ -41956,7 +42585,7 @@
         <v>734</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>1788</v>
+        <v>1829</v>
       </c>
       <c r="C735" s="2"/>
       <c r="D735" s="2"/>
@@ -41989,7 +42618,7 @@
         <v>735</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>1789</v>
+        <v>1830</v>
       </c>
       <c r="C736" s="2"/>
       <c r="D736" s="2"/>
@@ -42022,7 +42651,7 @@
         <v>736</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>1790</v>
+        <v>1831</v>
       </c>
       <c r="C737" s="2"/>
       <c r="D737" s="2"/>
@@ -42055,7 +42684,7 @@
         <v>737</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>1791</v>
+        <v>1832</v>
       </c>
       <c r="C738" s="2"/>
       <c r="D738" s="2"/>
@@ -42088,7 +42717,7 @@
         <v>738</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>1792</v>
+        <v>1833</v>
       </c>
       <c r="C739" s="2"/>
       <c r="D739" s="2"/>
@@ -42121,7 +42750,7 @@
         <v>739</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>1793</v>
+        <v>1834</v>
       </c>
       <c r="C740" s="2"/>
       <c r="D740" s="2"/>
@@ -42154,7 +42783,7 @@
         <v>740</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>1794</v>
+        <v>1835</v>
       </c>
       <c r="C741" s="2"/>
       <c r="D741" s="2"/>
@@ -42187,7 +42816,7 @@
         <v>741</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>1795</v>
+        <v>1836</v>
       </c>
       <c r="C742" s="2"/>
       <c r="D742" s="2"/>
@@ -42220,7 +42849,7 @@
         <v>742</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>1796</v>
+        <v>1837</v>
       </c>
       <c r="C743" s="2"/>
       <c r="D743" s="2"/>
@@ -42253,7 +42882,7 @@
         <v>743</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>1797</v>
+        <v>1838</v>
       </c>
       <c r="C744" s="2"/>
       <c r="D744" s="2"/>
@@ -42286,7 +42915,7 @@
         <v>744</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1798</v>
+        <v>1839</v>
       </c>
       <c r="C745" s="2"/>
       <c r="D745" s="2"/>
@@ -42319,7 +42948,7 @@
         <v>745</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>1799</v>
+        <v>1840</v>
       </c>
       <c r="C746" s="2"/>
       <c r="D746" s="2"/>
@@ -42352,7 +42981,7 @@
         <v>746</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>1800</v>
+        <v>1841</v>
       </c>
       <c r="C747" s="2"/>
       <c r="D747" s="2"/>
@@ -42385,7 +43014,7 @@
         <v>747</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>1801</v>
+        <v>1842</v>
       </c>
       <c r="C748" s="2"/>
       <c r="D748" s="2"/>
@@ -42418,7 +43047,7 @@
         <v>748</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1802</v>
+        <v>1843</v>
       </c>
       <c r="C749" s="2"/>
       <c r="D749" s="2"/>
@@ -42451,7 +43080,7 @@
         <v>749</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1803</v>
+        <v>1844</v>
       </c>
       <c r="C750" s="2"/>
       <c r="D750" s="2"/>
@@ -42484,7 +43113,7 @@
         <v>750</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1804</v>
+        <v>1845</v>
       </c>
       <c r="C751" s="2"/>
       <c r="D751" s="2"/>
@@ -42517,7 +43146,7 @@
         <v>751</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>1805</v>
+        <v>1846</v>
       </c>
       <c r="C752" s="2"/>
       <c r="D752" s="2"/>
@@ -42550,7 +43179,7 @@
         <v>752</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>1806</v>
+        <v>1847</v>
       </c>
       <c r="C753" s="2"/>
       <c r="D753" s="2"/>
@@ -42583,7 +43212,7 @@
         <v>753</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>1807</v>
+        <v>1848</v>
       </c>
       <c r="C754" s="2"/>
       <c r="D754" s="2"/>
@@ -42616,7 +43245,7 @@
         <v>754</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>1808</v>
+        <v>1849</v>
       </c>
       <c r="C755" s="2"/>
       <c r="D755" s="2"/>
@@ -42649,7 +43278,7 @@
         <v>755</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>1809</v>
+        <v>1850</v>
       </c>
       <c r="C756" s="2"/>
       <c r="D756" s="2"/>
@@ -42682,7 +43311,7 @@
         <v>756</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>1810</v>
+        <v>1851</v>
       </c>
       <c r="C757" s="2"/>
       <c r="D757" s="2"/>
@@ -42715,7 +43344,7 @@
         <v>757</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>1811</v>
+        <v>1852</v>
       </c>
       <c r="C758" s="2"/>
       <c r="D758" s="2"/>
@@ -42748,7 +43377,7 @@
         <v>758</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>1812</v>
+        <v>1853</v>
       </c>
       <c r="C759" s="2"/>
       <c r="D759" s="2"/>
@@ -42781,7 +43410,7 @@
         <v>759</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>1813</v>
+        <v>1854</v>
       </c>
       <c r="C760" s="2"/>
       <c r="D760" s="2"/>
@@ -42814,7 +43443,7 @@
         <v>760</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>1814</v>
+        <v>1855</v>
       </c>
       <c r="C761" s="2"/>
       <c r="D761" s="2"/>
@@ -42847,7 +43476,7 @@
         <v>761</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>1815</v>
+        <v>1856</v>
       </c>
       <c r="C762" s="2"/>
       <c r="D762" s="2"/>
@@ -42880,7 +43509,7 @@
         <v>762</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>1816</v>
+        <v>1857</v>
       </c>
       <c r="C763" s="2"/>
       <c r="D763" s="2"/>
@@ -42913,7 +43542,7 @@
         <v>763</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>1817</v>
+        <v>1858</v>
       </c>
       <c r="C764" s="2"/>
       <c r="D764" s="2"/>
@@ -42946,7 +43575,7 @@
         <v>764</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>1818</v>
+        <v>1859</v>
       </c>
       <c r="C765" s="2"/>
       <c r="D765" s="2"/>
@@ -42979,7 +43608,7 @@
         <v>765</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>1819</v>
+        <v>1860</v>
       </c>
       <c r="C766" s="2"/>
       <c r="D766" s="2"/>
@@ -43012,7 +43641,7 @@
         <v>766</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>1820</v>
+        <v>1861</v>
       </c>
       <c r="C767" s="2"/>
       <c r="D767" s="2"/>
@@ -43045,7 +43674,7 @@
         <v>767</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>1821</v>
+        <v>1862</v>
       </c>
       <c r="C768" s="2"/>
       <c r="D768" s="2"/>
@@ -43078,7 +43707,7 @@
         <v>768</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>1822</v>
+        <v>1863</v>
       </c>
       <c r="C769" s="2"/>
       <c r="D769" s="2"/>
@@ -43111,7 +43740,7 @@
         <v>769</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>1823</v>
+        <v>1864</v>
       </c>
       <c r="C770" s="2"/>
       <c r="D770" s="2"/>
@@ -43144,7 +43773,7 @@
         <v>770</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>1824</v>
+        <v>1865</v>
       </c>
       <c r="C771" s="2"/>
       <c r="D771" s="2"/>
@@ -43177,7 +43806,7 @@
         <v>771</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>1825</v>
+        <v>1866</v>
       </c>
       <c r="C772" s="2"/>
       <c r="D772" s="2"/>
@@ -43210,7 +43839,7 @@
         <v>772</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>1826</v>
+        <v>1867</v>
       </c>
       <c r="C773" s="2"/>
       <c r="D773" s="2"/>
@@ -43243,7 +43872,7 @@
         <v>773</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>1827</v>
+        <v>1868</v>
       </c>
       <c r="C774" s="2"/>
       <c r="D774" s="2"/>
@@ -43276,7 +43905,7 @@
         <v>774</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>1828</v>
+        <v>1869</v>
       </c>
       <c r="C775" s="2"/>
       <c r="D775" s="2"/>
@@ -43309,7 +43938,7 @@
         <v>775</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>1829</v>
+        <v>1870</v>
       </c>
       <c r="C776" s="2"/>
       <c r="D776" s="2"/>
@@ -43342,7 +43971,7 @@
         <v>776</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>1830</v>
+        <v>1871</v>
       </c>
       <c r="C777" s="2"/>
       <c r="D777" s="2"/>
@@ -43375,7 +44004,7 @@
         <v>777</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>1831</v>
+        <v>1872</v>
       </c>
       <c r="C778" s="2"/>
       <c r="D778" s="2"/>
@@ -43408,7 +44037,7 @@
         <v>778</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>1832</v>
+        <v>1873</v>
       </c>
       <c r="C779" s="2"/>
       <c r="D779" s="2"/>
@@ -43441,7 +44070,7 @@
         <v>779</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>1833</v>
+        <v>1874</v>
       </c>
       <c r="C780" s="2"/>
       <c r="D780" s="2"/>
@@ -43474,7 +44103,7 @@
         <v>780</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>1834</v>
+        <v>1875</v>
       </c>
       <c r="C781" s="2"/>
       <c r="D781" s="2"/>
@@ -43507,7 +44136,7 @@
         <v>781</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>1835</v>
+        <v>1876</v>
       </c>
       <c r="C782" s="2"/>
       <c r="D782" s="2"/>
@@ -43540,7 +44169,7 @@
         <v>782</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>1836</v>
+        <v>1877</v>
       </c>
       <c r="C783" s="2"/>
       <c r="D783" s="2"/>
@@ -43573,7 +44202,7 @@
         <v>783</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>1837</v>
+        <v>1878</v>
       </c>
       <c r="C784" s="2"/>
       <c r="D784" s="2"/>
@@ -43606,7 +44235,7 @@
         <v>784</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>1838</v>
+        <v>1879</v>
       </c>
       <c r="C785" s="2"/>
       <c r="D785" s="2"/>
@@ -43639,7 +44268,7 @@
         <v>785</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>1839</v>
+        <v>1880</v>
       </c>
       <c r="C786" s="2"/>
       <c r="D786" s="2"/>
@@ -43672,7 +44301,7 @@
         <v>786</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>1840</v>
+        <v>1881</v>
       </c>
       <c r="C787" s="2"/>
       <c r="D787" s="2"/>
@@ -43705,7 +44334,7 @@
         <v>787</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>1841</v>
+        <v>1882</v>
       </c>
       <c r="C788" s="2"/>
       <c r="D788" s="2"/>
@@ -43738,7 +44367,7 @@
         <v>788</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>1842</v>
+        <v>1883</v>
       </c>
       <c r="C789" s="2"/>
       <c r="D789" s="2"/>
@@ -43771,7 +44400,7 @@
         <v>789</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>1843</v>
+        <v>1884</v>
       </c>
       <c r="C790" s="2"/>
       <c r="D790" s="2"/>
@@ -43804,7 +44433,7 @@
         <v>790</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>1844</v>
+        <v>1885</v>
       </c>
       <c r="C791" s="2"/>
       <c r="D791" s="2"/>
@@ -43837,7 +44466,7 @@
         <v>791</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>1845</v>
+        <v>1886</v>
       </c>
       <c r="C792" s="2"/>
       <c r="D792" s="2"/>
@@ -43870,7 +44499,7 @@
         <v>792</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>1846</v>
+        <v>1887</v>
       </c>
       <c r="C793" s="2"/>
       <c r="D793" s="2"/>
@@ -43903,7 +44532,7 @@
         <v>793</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>1847</v>
+        <v>1888</v>
       </c>
       <c r="C794" s="2"/>
       <c r="D794" s="2"/>
@@ -43936,7 +44565,7 @@
         <v>794</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>1848</v>
+        <v>1889</v>
       </c>
       <c r="C795" s="2"/>
       <c r="D795" s="2"/>
@@ -43969,7 +44598,7 @@
         <v>795</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>1849</v>
+        <v>1890</v>
       </c>
       <c r="C796" s="2"/>
       <c r="D796" s="2"/>
@@ -44002,7 +44631,7 @@
         <v>796</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>1850</v>
+        <v>1891</v>
       </c>
       <c r="C797" s="2"/>
       <c r="D797" s="2"/>
@@ -44035,7 +44664,7 @@
         <v>797</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>1851</v>
+        <v>1892</v>
       </c>
       <c r="C798" s="2"/>
       <c r="D798" s="2"/>
@@ -44068,7 +44697,7 @@
         <v>798</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>1852</v>
+        <v>1893</v>
       </c>
       <c r="C799" s="2"/>
       <c r="D799" s="2"/>
@@ -44101,7 +44730,7 @@
         <v>799</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>1853</v>
+        <v>1894</v>
       </c>
       <c r="C800" s="2"/>
       <c r="D800" s="2"/>
@@ -44134,7 +44763,7 @@
         <v>800</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>1854</v>
+        <v>1895</v>
       </c>
       <c r="C801" s="2"/>
       <c r="D801" s="2"/>
@@ -44167,7 +44796,7 @@
         <v>801</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>1855</v>
+        <v>1896</v>
       </c>
       <c r="C802" s="2"/>
       <c r="D802" s="2"/>
@@ -44200,7 +44829,7 @@
         <v>802</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>1856</v>
+        <v>1897</v>
       </c>
       <c r="C803" s="2"/>
       <c r="D803" s="2"/>
@@ -44233,7 +44862,7 @@
         <v>803</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>1857</v>
+        <v>1898</v>
       </c>
       <c r="C804" s="2"/>
       <c r="D804" s="2"/>
@@ -44266,7 +44895,7 @@
         <v>804</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>1858</v>
+        <v>1899</v>
       </c>
       <c r="C805" s="2"/>
       <c r="D805" s="2"/>
@@ -44299,7 +44928,7 @@
         <v>805</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>1859</v>
+        <v>1900</v>
       </c>
       <c r="C806" s="2"/>
       <c r="D806" s="2"/>
@@ -44332,7 +44961,7 @@
         <v>806</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>1860</v>
+        <v>1901</v>
       </c>
       <c r="C807" s="2"/>
       <c r="D807" s="2"/>
@@ -44365,7 +44994,7 @@
         <v>807</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>1861</v>
+        <v>1902</v>
       </c>
       <c r="C808" s="2"/>
       <c r="D808" s="2"/>
@@ -44398,7 +45027,7 @@
         <v>808</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>1862</v>
+        <v>1903</v>
       </c>
       <c r="C809" s="2"/>
       <c r="D809" s="2"/>
@@ -44431,7 +45060,7 @@
         <v>809</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>1863</v>
+        <v>1904</v>
       </c>
       <c r="C810" s="2"/>
       <c r="D810" s="2"/>
@@ -44464,7 +45093,7 @@
         <v>810</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>1864</v>
+        <v>1905</v>
       </c>
       <c r="C811" s="2"/>
       <c r="D811" s="2"/>
@@ -44497,7 +45126,7 @@
         <v>811</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>1865</v>
+        <v>1906</v>
       </c>
       <c r="C812" s="2"/>
       <c r="D812" s="2"/>
@@ -44530,7 +45159,7 @@
         <v>812</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>1866</v>
+        <v>1907</v>
       </c>
       <c r="C813" s="2"/>
       <c r="D813" s="2"/>
@@ -44563,7 +45192,7 @@
         <v>813</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>1867</v>
+        <v>1908</v>
       </c>
       <c r="C814" s="2"/>
       <c r="D814" s="2"/>
@@ -44596,7 +45225,7 @@
         <v>814</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>1868</v>
+        <v>1909</v>
       </c>
       <c r="C815" s="2"/>
       <c r="D815" s="2"/>
@@ -44629,7 +45258,7 @@
         <v>815</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>1869</v>
+        <v>1910</v>
       </c>
       <c r="C816" s="2"/>
       <c r="D816" s="2"/>
@@ -44662,7 +45291,7 @@
         <v>816</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>1870</v>
+        <v>1911</v>
       </c>
       <c r="C817" s="2"/>
       <c r="D817" s="2"/>
@@ -44695,7 +45324,7 @@
         <v>817</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>1871</v>
+        <v>1912</v>
       </c>
       <c r="C818" s="2"/>
       <c r="D818" s="2"/>
@@ -44728,7 +45357,7 @@
         <v>818</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>1872</v>
+        <v>1913</v>
       </c>
       <c r="C819" s="2"/>
       <c r="D819" s="2"/>
@@ -44761,7 +45390,7 @@
         <v>819</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>1873</v>
+        <v>1914</v>
       </c>
       <c r="C820" s="2"/>
       <c r="D820" s="2"/>
@@ -44794,7 +45423,7 @@
         <v>820</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>1874</v>
+        <v>1915</v>
       </c>
       <c r="C821" s="2"/>
       <c r="D821" s="2"/>
@@ -44827,7 +45456,7 @@
         <v>821</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>1875</v>
+        <v>1916</v>
       </c>
       <c r="C822" s="2"/>
       <c r="D822" s="2"/>
@@ -44860,7 +45489,7 @@
         <v>822</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>1876</v>
+        <v>1917</v>
       </c>
       <c r="C823" s="2"/>
       <c r="D823" s="2"/>
@@ -44893,7 +45522,7 @@
         <v>823</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>1877</v>
+        <v>1918</v>
       </c>
       <c r="C824" s="2"/>
       <c r="D824" s="2"/>
@@ -44926,7 +45555,7 @@
         <v>824</v>
       </c>
       <c r="B825" s="2" t="s">
-        <v>1878</v>
+        <v>1919</v>
       </c>
       <c r="C825" s="2"/>
       <c r="D825" s="2"/>
@@ -44959,7 +45588,7 @@
         <v>825</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>1879</v>
+        <v>1920</v>
       </c>
       <c r="C826" s="2"/>
       <c r="D826" s="2"/>
@@ -44992,7 +45621,7 @@
         <v>826</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>1880</v>
+        <v>1921</v>
       </c>
       <c r="C827" s="2"/>
       <c r="D827" s="2"/>
@@ -45025,7 +45654,7 @@
         <v>827</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>1881</v>
+        <v>1922</v>
       </c>
       <c r="C828" s="2"/>
       <c r="D828" s="2"/>
@@ -45058,7 +45687,7 @@
         <v>828</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>1882</v>
+        <v>1923</v>
       </c>
       <c r="C829" s="2"/>
       <c r="D829" s="2"/>
@@ -45091,7 +45720,7 @@
         <v>829</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>1883</v>
+        <v>1924</v>
       </c>
       <c r="C830" s="2"/>
       <c r="D830" s="2"/>
@@ -45124,7 +45753,7 @@
         <v>830</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>1884</v>
+        <v>1925</v>
       </c>
       <c r="C831" s="2"/>
       <c r="D831" s="2"/>
@@ -45157,7 +45786,7 @@
         <v>831</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>1885</v>
+        <v>1926</v>
       </c>
       <c r="C832" s="2"/>
       <c r="D832" s="2"/>
@@ -45190,7 +45819,7 @@
         <v>832</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>1886</v>
+        <v>1927</v>
       </c>
       <c r="C833" s="2"/>
       <c r="D833" s="2"/>
@@ -45223,7 +45852,7 @@
         <v>833</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>1887</v>
+        <v>1928</v>
       </c>
       <c r="C834" s="2"/>
       <c r="D834" s="2"/>
@@ -45256,7 +45885,7 @@
         <v>834</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>1888</v>
+        <v>1929</v>
       </c>
       <c r="C835" s="2"/>
       <c r="D835" s="2"/>
@@ -45289,7 +45918,7 @@
         <v>835</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>1889</v>
+        <v>1930</v>
       </c>
       <c r="C836" s="2"/>
       <c r="D836" s="2"/>
@@ -45322,7 +45951,7 @@
         <v>836</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>1890</v>
+        <v>1931</v>
       </c>
       <c r="C837" s="2"/>
       <c r="D837" s="2"/>
@@ -45355,7 +45984,7 @@
         <v>837</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>1891</v>
+        <v>1932</v>
       </c>
       <c r="C838" s="2"/>
       <c r="D838" s="2"/>
@@ -45388,7 +46017,7 @@
         <v>838</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>1892</v>
+        <v>1933</v>
       </c>
       <c r="C839" s="2"/>
       <c r="D839" s="2"/>
@@ -45421,7 +46050,7 @@
         <v>839</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>1893</v>
+        <v>1934</v>
       </c>
       <c r="C840" s="2"/>
       <c r="D840" s="2"/>
@@ -45454,7 +46083,7 @@
         <v>840</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>1894</v>
+        <v>1935</v>
       </c>
       <c r="C841" s="2"/>
       <c r="D841" s="2"/>
@@ -45487,7 +46116,7 @@
         <v>841</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>1895</v>
+        <v>1936</v>
       </c>
       <c r="C842" s="2"/>
       <c r="D842" s="2"/>
@@ -45520,7 +46149,7 @@
         <v>842</v>
       </c>
       <c r="B843" s="2" t="s">
-        <v>1896</v>
+        <v>1937</v>
       </c>
       <c r="C843" s="2"/>
       <c r="D843" s="2"/>
@@ -45553,7 +46182,7 @@
         <v>843</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>1897</v>
+        <v>1938</v>
       </c>
       <c r="C844" s="2"/>
       <c r="D844" s="2"/>
@@ -45586,7 +46215,7 @@
         <v>844</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>1898</v>
+        <v>1939</v>
       </c>
       <c r="C845" s="2"/>
       <c r="D845" s="2"/>
@@ -45619,7 +46248,7 @@
         <v>845</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>1899</v>
+        <v>1940</v>
       </c>
       <c r="C846" s="2"/>
       <c r="D846" s="2"/>
@@ -45652,7 +46281,7 @@
         <v>846</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>1900</v>
+        <v>1941</v>
       </c>
       <c r="C847" s="2"/>
       <c r="D847" s="2"/>
@@ -45685,7 +46314,7 @@
         <v>847</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>1901</v>
+        <v>1942</v>
       </c>
       <c r="C848" s="2"/>
       <c r="D848" s="2"/>
@@ -45718,7 +46347,7 @@
         <v>848</v>
       </c>
       <c r="B849" s="2" t="s">
-        <v>1902</v>
+        <v>1943</v>
       </c>
       <c r="C849" s="2"/>
       <c r="D849" s="2"/>
@@ -45751,7 +46380,7 @@
         <v>849</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>1903</v>
+        <v>1944</v>
       </c>
       <c r="C850" s="2"/>
       <c r="D850" s="2"/>
@@ -45784,7 +46413,7 @@
         <v>850</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>1904</v>
+        <v>1945</v>
       </c>
       <c r="C851" s="2"/>
       <c r="D851" s="2"/>
@@ -45817,7 +46446,7 @@
         <v>851</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>1905</v>
+        <v>1946</v>
       </c>
       <c r="C852" s="2"/>
       <c r="D852" s="2"/>
@@ -45850,7 +46479,7 @@
         <v>852</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>1906</v>
+        <v>1947</v>
       </c>
       <c r="C853" s="2"/>
       <c r="D853" s="2"/>
@@ -45883,7 +46512,7 @@
         <v>853</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>1907</v>
+        <v>1948</v>
       </c>
       <c r="C854" s="2"/>
       <c r="D854" s="2"/>
@@ -45916,7 +46545,7 @@
         <v>854</v>
       </c>
       <c r="B855" s="2" t="s">
-        <v>1908</v>
+        <v>1949</v>
       </c>
       <c r="C855" s="2"/>
       <c r="D855" s="2"/>
@@ -45949,7 +46578,7 @@
         <v>855</v>
       </c>
       <c r="B856" s="2" t="s">
-        <v>1909</v>
+        <v>1950</v>
       </c>
       <c r="C856" s="2"/>
       <c r="D856" s="2"/>
@@ -45982,7 +46611,7 @@
         <v>856</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>1910</v>
+        <v>1951</v>
       </c>
       <c r="C857" s="2"/>
       <c r="D857" s="2"/>
@@ -46015,7 +46644,7 @@
         <v>857</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>1911</v>
+        <v>1952</v>
       </c>
       <c r="C858" s="2"/>
       <c r="D858" s="2"/>
@@ -46048,7 +46677,7 @@
         <v>858</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>1912</v>
+        <v>1953</v>
       </c>
       <c r="C859" s="2"/>
       <c r="D859" s="2"/>
@@ -46081,7 +46710,7 @@
         <v>859</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>1913</v>
+        <v>1954</v>
       </c>
       <c r="C860" s="2"/>
       <c r="D860" s="2"/>
@@ -46114,7 +46743,7 @@
         <v>860</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>1914</v>
+        <v>1955</v>
       </c>
       <c r="C861" s="2"/>
       <c r="D861" s="2"/>
@@ -46147,7 +46776,7 @@
         <v>861</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>1915</v>
+        <v>1956</v>
       </c>
       <c r="C862" s="2"/>
       <c r="D862" s="2"/>
@@ -46180,7 +46809,7 @@
         <v>862</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>1916</v>
+        <v>1957</v>
       </c>
       <c r="C863" s="2"/>
       <c r="D863" s="2"/>
@@ -46213,7 +46842,7 @@
         <v>863</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>1917</v>
+        <v>1958</v>
       </c>
       <c r="C864" s="2"/>
       <c r="D864" s="2"/>
@@ -46246,7 +46875,7 @@
         <v>864</v>
       </c>
       <c r="B865" s="2" t="s">
-        <v>1918</v>
+        <v>1959</v>
       </c>
       <c r="C865" s="2"/>
       <c r="D865" s="2"/>
@@ -46279,7 +46908,7 @@
         <v>865</v>
       </c>
       <c r="B866" s="2" t="s">
-        <v>1919</v>
+        <v>1960</v>
       </c>
       <c r="C866" s="2"/>
       <c r="D866" s="2"/>
@@ -46312,7 +46941,7 @@
         <v>866</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>1920</v>
+        <v>1961</v>
       </c>
       <c r="C867" s="2"/>
       <c r="D867" s="2"/>
@@ -46345,7 +46974,7 @@
         <v>867</v>
       </c>
       <c r="B868" s="2" t="s">
-        <v>1921</v>
+        <v>1962</v>
       </c>
       <c r="C868" s="2"/>
       <c r="D868" s="2"/>
@@ -46378,7 +47007,7 @@
         <v>868</v>
       </c>
       <c r="B869" s="2" t="s">
-        <v>1922</v>
+        <v>1963</v>
       </c>
       <c r="C869" s="2"/>
       <c r="D869" s="2"/>
@@ -46411,7 +47040,7 @@
         <v>869</v>
       </c>
       <c r="B870" s="2" t="s">
-        <v>1923</v>
+        <v>1964</v>
       </c>
       <c r="C870" s="2"/>
       <c r="D870" s="2"/>
@@ -46444,7 +47073,7 @@
         <v>870</v>
       </c>
       <c r="B871" s="2" t="s">
-        <v>1924</v>
+        <v>1965</v>
       </c>
       <c r="C871" s="2"/>
       <c r="D871" s="2"/>
@@ -46477,7 +47106,7 @@
         <v>871</v>
       </c>
       <c r="B872" s="2" t="s">
-        <v>1925</v>
+        <v>1966</v>
       </c>
       <c r="C872" s="2"/>
       <c r="D872" s="2"/>
@@ -46510,7 +47139,7 @@
         <v>872</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>1926</v>
+        <v>1967</v>
       </c>
       <c r="C873" s="2"/>
       <c r="D873" s="2"/>
@@ -46543,7 +47172,7 @@
         <v>873</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>1927</v>
+        <v>1968</v>
       </c>
       <c r="C874" s="2"/>
       <c r="D874" s="2"/>
@@ -46576,7 +47205,7 @@
         <v>874</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>1928</v>
+        <v>1969</v>
       </c>
       <c r="C875" s="2"/>
       <c r="D875" s="2"/>
@@ -46609,7 +47238,7 @@
         <v>875</v>
       </c>
       <c r="B876" s="2" t="s">
-        <v>1929</v>
+        <v>1970</v>
       </c>
       <c r="C876" s="2"/>
       <c r="D876" s="2"/>
@@ -46642,7 +47271,7 @@
         <v>876</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>1930</v>
+        <v>1971</v>
       </c>
       <c r="C877" s="2"/>
       <c r="D877" s="2"/>
@@ -46675,7 +47304,7 @@
         <v>877</v>
       </c>
       <c r="B878" s="2" t="s">
-        <v>1931</v>
+        <v>1972</v>
       </c>
       <c r="C878" s="2"/>
       <c r="D878" s="2"/>
@@ -46708,7 +47337,7 @@
         <v>878</v>
       </c>
       <c r="B879" s="2" t="s">
-        <v>1932</v>
+        <v>1973</v>
       </c>
       <c r="C879" s="2"/>
       <c r="D879" s="2"/>
@@ -46741,7 +47370,7 @@
         <v>879</v>
       </c>
       <c r="B880" s="2" t="s">
-        <v>1933</v>
+        <v>1974</v>
       </c>
       <c r="C880" s="2"/>
       <c r="D880" s="2"/>
@@ -46774,7 +47403,7 @@
         <v>880</v>
       </c>
       <c r="B881" s="2" t="s">
-        <v>1934</v>
+        <v>1975</v>
       </c>
       <c r="C881" s="2"/>
       <c r="D881" s="2"/>
@@ -46807,7 +47436,7 @@
         <v>881</v>
       </c>
       <c r="B882" s="2" t="s">
-        <v>1935</v>
+        <v>1976</v>
       </c>
       <c r="C882" s="2"/>
       <c r="D882" s="2"/>
@@ -46840,7 +47469,7 @@
         <v>882</v>
       </c>
       <c r="B883" s="2" t="s">
-        <v>1936</v>
+        <v>1977</v>
       </c>
       <c r="C883" s="2"/>
       <c r="D883" s="2"/>
@@ -46873,7 +47502,7 @@
         <v>883</v>
       </c>
       <c r="B884" s="2" t="s">
-        <v>1937</v>
+        <v>1978</v>
       </c>
       <c r="C884" s="2"/>
       <c r="D884" s="2"/>
@@ -46906,7 +47535,7 @@
         <v>884</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>1938</v>
+        <v>1979</v>
       </c>
       <c r="C885" s="2"/>
       <c r="D885" s="2"/>
@@ -46941,37 +47570,37 @@
         <v>885</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>1939</v>
+        <v>1980</v>
       </c>
       <c r="C886" t="s">
-        <v>1940</v>
+        <v>1981</v>
       </c>
       <c r="D886" s="2" t="s">
-        <v>1941</v>
+        <v>1982</v>
       </c>
       <c r="E886" s="2" t="s">
-        <v>1942</v>
+        <v>1983</v>
       </c>
       <c r="F886" s="2" t="s">
-        <v>1943</v>
+        <v>1984</v>
       </c>
       <c r="G886" s="2" t="s">
-        <v>1944</v>
+        <v>1985</v>
       </c>
       <c r="H886" s="2" t="s">
-        <v>1945</v>
+        <v>1986</v>
       </c>
       <c r="I886" s="2" t="s">
-        <v>1946</v>
+        <v>1987</v>
       </c>
       <c r="J886" s="2" t="s">
-        <v>1947</v>
+        <v>1988</v>
       </c>
       <c r="K886" s="2" t="s">
-        <v>1948</v>
+        <v>1989</v>
       </c>
       <c r="L886" s="2" t="s">
-        <v>1949</v>
+        <v>1990</v>
       </c>
       <c r="M886" s="2"/>
       <c r="N886" s="2"/>
@@ -46994,7 +47623,7 @@
         <v>886</v>
       </c>
       <c r="B887" s="2" t="s">
-        <v>1950</v>
+        <v>1991</v>
       </c>
       <c r="C887" s="2"/>
       <c r="D887" s="2"/>
@@ -47027,7 +47656,7 @@
         <v>887</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>1951</v>
+        <v>1992</v>
       </c>
       <c r="C888" s="2"/>
       <c r="D888" s="2"/>
@@ -47060,7 +47689,7 @@
         <v>888</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>1952</v>
+        <v>1993</v>
       </c>
       <c r="C889" s="2"/>
       <c r="D889" s="2"/>
@@ -47093,7 +47722,7 @@
         <v>889</v>
       </c>
       <c r="B890" s="2" t="s">
-        <v>1953</v>
+        <v>1994</v>
       </c>
       <c r="C890" s="2"/>
       <c r="D890" s="2"/>
@@ -47126,7 +47755,7 @@
         <v>890</v>
       </c>
       <c r="B891" s="2" t="s">
-        <v>1954</v>
+        <v>1995</v>
       </c>
       <c r="C891" s="2"/>
       <c r="D891" s="2"/>
@@ -47159,7 +47788,7 @@
         <v>891</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>1955</v>
+        <v>1996</v>
       </c>
       <c r="C892" s="2"/>
       <c r="D892" s="2"/>
@@ -47192,7 +47821,7 @@
         <v>892</v>
       </c>
       <c r="B893" s="2" t="s">
-        <v>1956</v>
+        <v>1997</v>
       </c>
       <c r="C893" s="2"/>
       <c r="D893" s="2"/>
@@ -47225,7 +47854,7 @@
         <v>893</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>1957</v>
+        <v>1998</v>
       </c>
       <c r="C894" s="2"/>
       <c r="D894" s="2"/>
@@ -47258,7 +47887,7 @@
         <v>894</v>
       </c>
       <c r="B895" s="2" t="s">
-        <v>1958</v>
+        <v>1999</v>
       </c>
       <c r="C895" s="2"/>
       <c r="D895" s="2"/>
@@ -47291,7 +47920,7 @@
         <v>895</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>1959</v>
+        <v>2000</v>
       </c>
       <c r="C896" s="2"/>
       <c r="D896" s="2"/>
@@ -47324,7 +47953,7 @@
         <v>896</v>
       </c>
       <c r="B897" s="2" t="s">
-        <v>1960</v>
+        <v>2001</v>
       </c>
       <c r="C897" s="2"/>
       <c r="D897" s="2"/>
@@ -47357,7 +47986,7 @@
         <v>897</v>
       </c>
       <c r="B898" s="2" t="s">
-        <v>1961</v>
+        <v>2002</v>
       </c>
       <c r="C898" s="2"/>
       <c r="D898" s="2"/>
@@ -47390,7 +48019,7 @@
         <v>898</v>
       </c>
       <c r="B899" s="2" t="s">
-        <v>1962</v>
+        <v>2003</v>
       </c>
       <c r="C899" s="2"/>
       <c r="D899" s="2"/>
@@ -47423,7 +48052,7 @@
         <v>899</v>
       </c>
       <c r="B900" s="2" t="s">
-        <v>1963</v>
+        <v>2004</v>
       </c>
       <c r="C900" s="2"/>
       <c r="D900" s="2"/>
@@ -47456,7 +48085,7 @@
         <v>900</v>
       </c>
       <c r="B901" s="2" t="s">
-        <v>1964</v>
+        <v>2005</v>
       </c>
       <c r="C901" s="2"/>
       <c r="D901" s="2"/>
@@ -47489,7 +48118,7 @@
         <v>901</v>
       </c>
       <c r="B902" s="2" t="s">
-        <v>1965</v>
+        <v>2006</v>
       </c>
       <c r="C902" s="2"/>
       <c r="D902" s="2"/>
@@ -47522,7 +48151,7 @@
         <v>902</v>
       </c>
       <c r="B903" s="2" t="s">
-        <v>1966</v>
+        <v>2007</v>
       </c>
       <c r="C903" s="2"/>
       <c r="D903" s="2"/>
@@ -47555,7 +48184,7 @@
         <v>903</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>1967</v>
+        <v>2008</v>
       </c>
       <c r="C904" s="2"/>
       <c r="D904" s="2"/>
@@ -47588,7 +48217,7 @@
         <v>904</v>
       </c>
       <c r="B905" s="2" t="s">
-        <v>1968</v>
+        <v>2009</v>
       </c>
       <c r="C905" s="2"/>
       <c r="D905" s="2"/>
@@ -47621,7 +48250,7 @@
         <v>905</v>
       </c>
       <c r="B906" s="2" t="s">
-        <v>1969</v>
+        <v>2010</v>
       </c>
       <c r="C906" s="2"/>
       <c r="D906" s="2"/>
@@ -47654,7 +48283,7 @@
         <v>906</v>
       </c>
       <c r="B907" s="2" t="s">
-        <v>1970</v>
+        <v>2011</v>
       </c>
       <c r="C907" s="2"/>
       <c r="D907" s="2"/>
@@ -47687,7 +48316,7 @@
         <v>907</v>
       </c>
       <c r="B908" s="2" t="s">
-        <v>1971</v>
+        <v>2012</v>
       </c>
       <c r="C908" s="2"/>
       <c r="D908" s="2"/>
@@ -47720,7 +48349,7 @@
         <v>908</v>
       </c>
       <c r="B909" s="2" t="s">
-        <v>1972</v>
+        <v>2013</v>
       </c>
       <c r="C909" s="2"/>
       <c r="D909" s="2"/>
@@ -47753,7 +48382,7 @@
         <v>909</v>
       </c>
       <c r="B910" s="2" t="s">
-        <v>1973</v>
+        <v>2014</v>
       </c>
       <c r="C910" s="2"/>
       <c r="D910" s="2"/>
@@ -47786,7 +48415,7 @@
         <v>910</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>1974</v>
+        <v>2015</v>
       </c>
       <c r="C911" s="2"/>
       <c r="D911" s="2"/>
@@ -47819,7 +48448,7 @@
         <v>911</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>1975</v>
+        <v>2016</v>
       </c>
       <c r="C912" s="2"/>
       <c r="D912" s="2"/>
@@ -47852,37 +48481,37 @@
         <v>912</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>1976</v>
+        <v>2017</v>
       </c>
       <c r="C913" s="2" t="s">
-        <v>1977</v>
+        <v>2018</v>
       </c>
       <c r="D913" s="2" t="s">
-        <v>1978</v>
+        <v>2019</v>
       </c>
       <c r="E913" s="2" t="s">
-        <v>1979</v>
+        <v>2020</v>
       </c>
       <c r="F913" s="2" t="s">
-        <v>1980</v>
+        <v>2021</v>
       </c>
       <c r="G913" s="2" t="s">
-        <v>1981</v>
+        <v>2022</v>
       </c>
       <c r="H913" s="2" t="s">
-        <v>1982</v>
+        <v>2023</v>
       </c>
       <c r="I913" s="2" t="s">
-        <v>1983</v>
+        <v>2024</v>
       </c>
       <c r="J913" s="2" t="s">
-        <v>1984</v>
+        <v>2025</v>
       </c>
       <c r="K913" s="2" t="s">
-        <v>1985</v>
+        <v>2026</v>
       </c>
       <c r="L913" s="2" t="s">
-        <v>1986</v>
+        <v>2027</v>
       </c>
       <c r="M913" s="2"/>
       <c r="N913" s="2"/>
@@ -47905,7 +48534,7 @@
         <v>913</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>1987</v>
+        <v>2028</v>
       </c>
       <c r="C914" s="2"/>
       <c r="D914" s="2"/>
@@ -47938,7 +48567,7 @@
         <v>914</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>1988</v>
+        <v>2029</v>
       </c>
       <c r="C915" s="2"/>
       <c r="D915" s="2"/>
@@ -47971,7 +48600,7 @@
         <v>915</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1989</v>
+        <v>2030</v>
       </c>
       <c r="C916" s="2"/>
       <c r="D916" s="2"/>
@@ -48004,7 +48633,7 @@
         <v>916</v>
       </c>
       <c r="B917" s="2" t="s">
-        <v>1990</v>
+        <v>2031</v>
       </c>
       <c r="C917" s="2"/>
       <c r="D917" s="2"/>
@@ -48037,7 +48666,7 @@
         <v>917</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1991</v>
+        <v>2032</v>
       </c>
       <c r="C918" s="2"/>
       <c r="D918" s="2"/>
@@ -48070,7 +48699,7 @@
         <v>918</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1992</v>
+        <v>2033</v>
       </c>
       <c r="C919" s="2"/>
       <c r="D919" s="2"/>
@@ -48103,7 +48732,7 @@
         <v>919</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>1993</v>
+        <v>2034</v>
       </c>
       <c r="C920" s="2"/>
       <c r="D920" s="2"/>
@@ -48136,7 +48765,7 @@
         <v>920</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>1994</v>
+        <v>2035</v>
       </c>
       <c r="C921" s="2"/>
       <c r="D921" s="2"/>
@@ -48169,7 +48798,7 @@
         <v>921</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>1995</v>
+        <v>2036</v>
       </c>
       <c r="C922" s="2"/>
       <c r="D922" s="2"/>
@@ -48202,7 +48831,7 @@
         <v>922</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1996</v>
+        <v>2037</v>
       </c>
       <c r="C923" s="2"/>
       <c r="D923" s="2"/>
@@ -48235,7 +48864,7 @@
         <v>923</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>1997</v>
+        <v>2038</v>
       </c>
       <c r="C924" s="2"/>
       <c r="D924" s="2"/>
@@ -48268,7 +48897,7 @@
         <v>924</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>1998</v>
+        <v>2039</v>
       </c>
       <c r="C925" s="2"/>
       <c r="D925" s="2"/>
@@ -48301,7 +48930,7 @@
         <v>925</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>1999</v>
+        <v>2040</v>
       </c>
       <c r="C926" s="2"/>
       <c r="D926" s="2"/>
@@ -48334,7 +48963,7 @@
         <v>926</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>2000</v>
+        <v>2041</v>
       </c>
       <c r="C927" s="2"/>
       <c r="D927" s="2"/>
@@ -48367,7 +48996,7 @@
         <v>927</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>2001</v>
+        <v>2042</v>
       </c>
       <c r="C928" s="2"/>
       <c r="D928" s="2"/>
@@ -48400,7 +49029,7 @@
         <v>928</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>2002</v>
+        <v>2043</v>
       </c>
       <c r="C929" s="2"/>
       <c r="D929" s="2"/>
@@ -48433,7 +49062,7 @@
         <v>929</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>2003</v>
+        <v>2044</v>
       </c>
       <c r="C930" s="2"/>
       <c r="D930" s="2"/>
@@ -48466,7 +49095,7 @@
         <v>930</v>
       </c>
       <c r="B931" s="2" t="s">
-        <v>2004</v>
+        <v>2045</v>
       </c>
       <c r="C931" s="2"/>
       <c r="D931" s="2"/>
@@ -48499,7 +49128,7 @@
         <v>931</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>2005</v>
+        <v>2046</v>
       </c>
       <c r="C932" s="2"/>
       <c r="D932" s="2"/>
@@ -48532,7 +49161,7 @@
         <v>932</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>2006</v>
+        <v>2047</v>
       </c>
       <c r="C933" s="2"/>
       <c r="D933" s="2"/>
@@ -48565,7 +49194,7 @@
         <v>933</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>2007</v>
+        <v>2048</v>
       </c>
       <c r="C934" s="2"/>
       <c r="D934" s="2"/>
@@ -48598,7 +49227,7 @@
         <v>934</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>2008</v>
+        <v>2049</v>
       </c>
       <c r="C935" s="2"/>
       <c r="D935" s="2"/>
@@ -48631,7 +49260,7 @@
         <v>935</v>
       </c>
       <c r="B936" s="2" t="s">
-        <v>2009</v>
+        <v>2050</v>
       </c>
       <c r="C936" s="2"/>
       <c r="D936" s="2"/>
@@ -48664,7 +49293,7 @@
         <v>936</v>
       </c>
       <c r="B937" s="2" t="s">
-        <v>2010</v>
+        <v>2051</v>
       </c>
       <c r="C937" s="2"/>
       <c r="D937" s="2"/>
@@ -48697,7 +49326,7 @@
         <v>937</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>2011</v>
+        <v>2052</v>
       </c>
       <c r="C938" s="2"/>
       <c r="D938" s="2"/>
@@ -48730,7 +49359,7 @@
         <v>938</v>
       </c>
       <c r="B939" s="2" t="s">
-        <v>2012</v>
+        <v>2053</v>
       </c>
       <c r="C939" s="2"/>
       <c r="D939" s="2"/>
@@ -48763,7 +49392,7 @@
         <v>939</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>2013</v>
+        <v>2054</v>
       </c>
       <c r="C940" s="2"/>
       <c r="D940" s="2"/>
@@ -48796,7 +49425,7 @@
         <v>940</v>
       </c>
       <c r="B941" s="2" t="s">
-        <v>2014</v>
+        <v>2055</v>
       </c>
       <c r="C941" s="2"/>
       <c r="D941" s="2"/>
@@ -48829,7 +49458,7 @@
         <v>941</v>
       </c>
       <c r="B942" s="2" t="s">
-        <v>2015</v>
+        <v>2056</v>
       </c>
       <c r="C942" s="2"/>
       <c r="D942" s="2"/>
@@ -48862,7 +49491,7 @@
         <v>942</v>
       </c>
       <c r="B943" s="2" t="s">
-        <v>2016</v>
+        <v>2057</v>
       </c>
       <c r="C943" s="2"/>
       <c r="D943" s="2"/>
@@ -48895,7 +49524,7 @@
         <v>943</v>
       </c>
       <c r="B944" s="2" t="s">
-        <v>2017</v>
+        <v>2058</v>
       </c>
       <c r="C944" s="2"/>
       <c r="D944" s="2"/>
@@ -48928,7 +49557,7 @@
         <v>944</v>
       </c>
       <c r="B945" s="2" t="s">
-        <v>2018</v>
+        <v>2059</v>
       </c>
       <c r="C945" s="2"/>
       <c r="D945" s="2"/>
@@ -48961,7 +49590,7 @@
         <v>945</v>
       </c>
       <c r="B946" s="2" t="s">
-        <v>2019</v>
+        <v>2060</v>
       </c>
       <c r="C946" s="2"/>
       <c r="D946" s="2"/>
@@ -48994,7 +49623,7 @@
         <v>946</v>
       </c>
       <c r="B947" s="2" t="s">
-        <v>2020</v>
+        <v>2061</v>
       </c>
       <c r="C947" s="2"/>
       <c r="D947" s="2"/>
@@ -49027,7 +49656,7 @@
         <v>947</v>
       </c>
       <c r="B948" s="2" t="s">
-        <v>2021</v>
+        <v>2062</v>
       </c>
       <c r="C948" s="2"/>
       <c r="D948" s="2"/>
@@ -49060,7 +49689,7 @@
         <v>948</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>2022</v>
+        <v>2063</v>
       </c>
       <c r="C949" s="2"/>
       <c r="D949" s="2"/>
@@ -49093,7 +49722,7 @@
         <v>949</v>
       </c>
       <c r="B950" s="2" t="s">
-        <v>2023</v>
+        <v>2064</v>
       </c>
       <c r="C950" s="2"/>
       <c r="D950" s="2"/>
@@ -49126,7 +49755,7 @@
         <v>950</v>
       </c>
       <c r="B951" s="2" t="s">
-        <v>2024</v>
+        <v>2065</v>
       </c>
       <c r="C951" s="2"/>
       <c r="D951" s="2"/>
@@ -49159,7 +49788,7 @@
         <v>951</v>
       </c>
       <c r="B952" s="2" t="s">
-        <v>2025</v>
+        <v>2066</v>
       </c>
       <c r="C952" s="2"/>
       <c r="D952" s="2"/>
@@ -49192,7 +49821,7 @@
         <v>952</v>
       </c>
       <c r="B953" s="2" t="s">
-        <v>2026</v>
+        <v>2067</v>
       </c>
       <c r="C953" s="2"/>
       <c r="D953" s="2"/>
@@ -49225,7 +49854,7 @@
         <v>953</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>2027</v>
+        <v>2068</v>
       </c>
       <c r="C954" s="2"/>
       <c r="D954" s="2"/>
@@ -49258,7 +49887,7 @@
         <v>954</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>2028</v>
+        <v>2069</v>
       </c>
       <c r="C955" s="2"/>
       <c r="D955" s="2"/>
@@ -49291,7 +49920,7 @@
         <v>955</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>2029</v>
+        <v>2070</v>
       </c>
       <c r="C956" s="2"/>
       <c r="D956" s="2"/>
@@ -49324,7 +49953,7 @@
         <v>956</v>
       </c>
       <c r="B957" s="2" t="s">
-        <v>2030</v>
+        <v>2071</v>
       </c>
       <c r="C957" s="2"/>
       <c r="D957" s="2"/>
@@ -49357,7 +49986,7 @@
         <v>957</v>
       </c>
       <c r="B958" s="2" t="s">
-        <v>2031</v>
+        <v>2072</v>
       </c>
       <c r="C958" s="2"/>
       <c r="D958" s="2"/>

</xml_diff>